<commit_message>
Inicio do projeto final
</commit_message>
<xml_diff>
--- a/NOTCH.xlsx
+++ b/NOTCH.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
   <si>
     <t>C=</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Reunião CÉ</t>
   </si>
   <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
     <t>Diabetes Miellitus</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>Processamento do sinal</t>
   </si>
   <si>
-    <t>Instrumentação (tipo de tratamento)</t>
-  </si>
-  <si>
     <t>Tipo de Hardware (justificativa)</t>
   </si>
   <si>
@@ -304,6 +298,9 @@
   </si>
   <si>
     <t>Disponibilização de dados</t>
+  </si>
+  <si>
+    <t>Instrumentação (tipo de tratamento do sinal)</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1197,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1248,13 +1245,13 @@
         <v>61</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1265,10 +1262,10 @@
         <v>63</v>
       </c>
       <c r="P2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1276,10 +1273,10 @@
         <v>64</v>
       </c>
       <c r="P3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1287,10 +1284,10 @@
         <v>65</v>
       </c>
       <c r="P4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1298,10 +1295,10 @@
         <v>66</v>
       </c>
       <c r="P5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1309,29 +1306,29 @@
         <v>67</v>
       </c>
       <c r="P6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="O7" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="P7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="O8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1339,47 +1336,42 @@
         <v>69</v>
       </c>
       <c r="P9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="O10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="15:15">
       <c r="O18" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="15:15">
       <c r="O19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="15:15">
       <c r="O20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="15:15">
       <c r="O21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="15:15">
       <c r="O22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="15:15">
       <c r="O24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="15:15">
       <c r="O25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>